<commit_message>
[Update] Actores y Diagrama de casos de uso
</commit_message>
<xml_diff>
--- a/análisis/Actores/Actor_Admin.xlsx
+++ b/análisis/Actores/Actor_Admin.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SyncHostel\synchostel\análisis\Actores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dvlpmnt\synchostel\análisis\Actores\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Actor</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Número telefónico del administrador</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -673,6 +676,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -688,66 +699,58 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1033,7 +1036,7 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1052,12 +1055,12 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1075,7 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
@@ -1084,7 +1087,7 @@
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1094,7 +1097,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="19"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
@@ -1104,50 +1107,50 @@
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="8"/>
       <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="9">
         <v>42112</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="21">
-        <v>1</v>
+      <c r="G7" s="34" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="29"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
@@ -1157,85 +1160,75 @@
         <v>17</v>
       </c>
       <c r="D11" s="18"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="18"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="11" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="18"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="19"/>
+      <c r="F13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="13" t="s">
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
     </row>
     <row r="17" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="28"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="C10:E10"/>
@@ -1244,6 +1237,16 @@
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>